<commit_message>
R12 Raw Data Imported
</commit_message>
<xml_diff>
--- a/THRef/A4_ThRef.xlsx
+++ b/THRef/A4_ThRef.xlsx
@@ -1,77 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_CF968E0DABCF094F20048FA27BED34BA348958A6" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{80E3B889-913B-4FD4-917A-6B43CB88E818}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="18195" windowHeight="6720"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="18195" windowHeight="6720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="56">
   <si>
     <t>Run #</t>
   </si>
   <si>
-    <t>Temp ©</t>
-  </si>
-  <si>
-    <t>pressure (gauge, kPA)</t>
-  </si>
-  <si>
-    <t>Current (A)</t>
-  </si>
-  <si>
-    <t>Evaporator</t>
-  </si>
-  <si>
-    <t>Motor</t>
-  </si>
-  <si>
-    <t>Condenser</t>
-  </si>
-  <si>
-    <t>Voltage (V)</t>
-  </si>
-  <si>
-    <t>Current  (A)</t>
-  </si>
-  <si>
-    <t>voltage  (V)</t>
-  </si>
-  <si>
-    <t>pressure  (gauge, kPA)</t>
-  </si>
-  <si>
-    <t>Rheostat  (%)</t>
-  </si>
-  <si>
-    <t>Force (N)</t>
-  </si>
-  <si>
-    <t>Speed (rpm)</t>
-  </si>
-  <si>
-    <t>Compressor Speed</t>
-  </si>
-  <si>
-    <t>Refrigerant</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>Mass flow rates (g/s</t>
-  </si>
-  <si>
     <t>Compressor Inlet 1</t>
   </si>
   <si>
@@ -123,17 +81,77 @@
     <t>8.18 cond</t>
   </si>
   <si>
-    <t>*decreasing</t>
-  </si>
-  <si>
-    <t>*increasing</t>
+    <t>Condenser pressure (gauge, kPA)</t>
+  </si>
+  <si>
+    <t>Condenser Rheostat  (%)</t>
+  </si>
+  <si>
+    <t>Evaporator pressure  (gauge, kPA)</t>
+  </si>
+  <si>
+    <t>Evaporator voltage  (V)</t>
+  </si>
+  <si>
+    <t>Evaporator Current  (A)</t>
+  </si>
+  <si>
+    <t>Motor Voltage (V)</t>
+  </si>
+  <si>
+    <t>Motor Current (A)</t>
+  </si>
+  <si>
+    <t>Motor Force (N)</t>
+  </si>
+  <si>
+    <t>Motor Speed (rpm)</t>
+  </si>
+  <si>
+    <t>Refrigerant Mass flow rate (g/s)</t>
+  </si>
+  <si>
+    <t>Water Mass flow rate (g/s)</t>
+  </si>
+  <si>
+    <t>Condenser Temp [C]</t>
+  </si>
+  <si>
+    <t>Compressor Speed [rpm]</t>
+  </si>
+  <si>
+    <t>Temperature Compressor Inlet 1</t>
+  </si>
+  <si>
+    <t>Temperature Compressor Outlet 2</t>
+  </si>
+  <si>
+    <t>Temperature CompressorOutlet 3</t>
+  </si>
+  <si>
+    <t>Temperature Throttle Valve Inlet 4</t>
+  </si>
+  <si>
+    <t>Temperature Evaporator Inlet 5</t>
+  </si>
+  <si>
+    <t>Temperature Evaporator Outlet 6</t>
+  </si>
+  <si>
+    <t>Temperature Water inlet 7</t>
+  </si>
+  <si>
+    <t>Temperature Water outlet 8</t>
+  </si>
+  <si>
+    <t>Run</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -199,20 +217,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -220,6 +235,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -266,7 +289,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -298,9 +321,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -332,6 +373,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -507,143 +566,248 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="E10" sqref="A1:V12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.91796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.796875" customWidth="1"/>
+    <col min="3" max="3" width="8.33984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.8359375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.98828125" customWidth="1"/>
+    <col min="6" max="6" width="10.76171875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.89453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28125" customWidth="1"/>
+    <col min="12" max="12" width="13.5859375" customWidth="1"/>
+    <col min="13" max="13" width="13.1796875" customWidth="1"/>
+    <col min="14" max="14" width="14.390625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="44.25" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="8" t="s">
+    <row r="1" spans="1:22" ht="68.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>800</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
+        <v>81.3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>140</v>
+      </c>
+      <c r="F2" s="2">
+        <v>80</v>
+      </c>
+      <c r="G2" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="H2" s="2">
+        <v>119</v>
+      </c>
+      <c r="I2" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="J2" s="2">
+        <v>9.75</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1767</v>
+      </c>
+      <c r="L2" s="2">
+        <v>461.3</v>
+      </c>
+      <c r="M2" s="2">
         <v>5</v>
       </c>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" ht="30">
-      <c r="A2" s="10"/>
-      <c r="B2" s="9" t="s">
+      <c r="N2" s="2">
+        <v>18</v>
+      </c>
+      <c r="O2">
+        <v>12.52</v>
+      </c>
+      <c r="P2">
+        <v>63.04</v>
+      </c>
+      <c r="Q2">
+        <v>22.33</v>
+      </c>
+      <c r="R2">
+        <v>22.45</v>
+      </c>
+      <c r="S2">
+        <v>-8.85</v>
+      </c>
+      <c r="T2">
+        <v>10.5</v>
+      </c>
+      <c r="U2">
+        <v>12.56</v>
+      </c>
+      <c r="V2">
+        <v>24.82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="B3" s="2">
+        <v>795</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
+        <v>75.5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>115</v>
+      </c>
+      <c r="F3" s="2">
+        <v>75</v>
+      </c>
+      <c r="G3" s="2">
+        <v>8.1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>118</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="J3" s="2">
         <v>9</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="9" t="s">
+      <c r="K3" s="2">
+        <v>1767</v>
+      </c>
+      <c r="L3" s="2">
+        <v>461.9</v>
+      </c>
+      <c r="M3" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="N3" s="2">
+        <v>17.5</v>
+      </c>
+      <c r="O3">
+        <v>11.25</v>
+      </c>
+      <c r="P3">
+        <v>65.010000000000005</v>
+      </c>
+      <c r="Q3">
+        <v>20.81</v>
+      </c>
+      <c r="R3">
+        <v>21.65</v>
+      </c>
+      <c r="S3">
+        <v>-11.91</v>
+      </c>
+      <c r="T3">
+        <v>7.82</v>
+      </c>
+      <c r="U3">
+        <v>12.64</v>
+      </c>
+      <c r="V3">
+        <v>23.79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
         <v>3</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2">
-        <v>80</v>
-      </c>
-      <c r="G3" s="2">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="H3" s="2">
-        <v>119</v>
-      </c>
-      <c r="I3" s="2">
-        <v>7.3</v>
-      </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="2">
-        <v>1</v>
       </c>
       <c r="B4" s="2">
         <v>800</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2">
-        <v>81.3</v>
+        <v>68.5</v>
       </c>
       <c r="E4" s="2">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="F4" s="2">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G4" s="2">
-        <v>8.9</v>
+        <v>7.4</v>
       </c>
       <c r="H4" s="2">
         <v>119</v>
@@ -652,407 +816,610 @@
         <v>7.2</v>
       </c>
       <c r="J4" s="2">
-        <v>9.75</v>
+        <v>8.5</v>
       </c>
       <c r="K4" s="2">
-        <v>1767</v>
+        <v>1770</v>
       </c>
       <c r="L4" s="2">
-        <v>461.3</v>
+        <v>461.45</v>
       </c>
       <c r="M4" s="2">
-        <v>5</v>
+        <v>3.75</v>
       </c>
       <c r="N4" s="2">
-        <v>18</v>
-      </c>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15">
+        <v>13.1</v>
+      </c>
+      <c r="O4">
+        <v>9.67</v>
+      </c>
+      <c r="P4">
+        <v>66.56</v>
+      </c>
+      <c r="Q4">
+        <v>20.72</v>
+      </c>
+      <c r="R4">
+        <v>21.37</v>
+      </c>
+      <c r="S4">
+        <v>-15.8</v>
+      </c>
+      <c r="T4">
+        <v>4.24</v>
+      </c>
+      <c r="U4">
+        <v>12.87</v>
+      </c>
+      <c r="V4">
+        <v>25.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>795</v>
+        <v>800</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2">
-        <v>75.5</v>
+        <v>61.5</v>
       </c>
       <c r="E5" s="2">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="F5" s="2">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G5" s="2">
-        <v>8.1</v>
+        <v>6.6</v>
       </c>
       <c r="H5" s="2">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I5" s="2">
         <v>7.2</v>
       </c>
       <c r="J5" s="2">
-        <v>9</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="K5" s="2">
-        <v>1767</v>
+        <v>1772</v>
       </c>
       <c r="L5" s="2">
-        <v>461.9</v>
+        <v>464.6</v>
       </c>
       <c r="M5" s="2">
-        <v>4.5</v>
+        <v>3.2</v>
       </c>
       <c r="N5" s="2">
-        <v>17.5</v>
-      </c>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15">
+        <v>10.5</v>
+      </c>
+      <c r="O5">
+        <v>8.31</v>
+      </c>
+      <c r="P5">
+        <v>67.510000000000005</v>
+      </c>
+      <c r="Q5">
+        <v>20.190000000000001</v>
+      </c>
+      <c r="R5">
+        <v>21.05</v>
+      </c>
+      <c r="S5">
+        <v>-19.239999999999998</v>
+      </c>
+      <c r="T5">
+        <v>1.05</v>
+      </c>
+      <c r="U5">
+        <v>13.09</v>
+      </c>
+      <c r="V5">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>800</v>
+        <v>810</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
-        <v>68.5</v>
+        <v>53</v>
       </c>
       <c r="E6" s="2">
-        <v>85</v>
+        <v>20.5</v>
       </c>
       <c r="F6" s="2">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="G6" s="2">
-        <v>7.4</v>
+        <v>5.75</v>
       </c>
       <c r="H6" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I6" s="2">
-        <v>7.2</v>
+        <v>7.15</v>
       </c>
       <c r="J6" s="2">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="K6" s="2">
-        <v>1770</v>
+        <v>1774</v>
       </c>
       <c r="L6" s="2">
-        <v>461.45</v>
+        <v>465.9</v>
       </c>
       <c r="M6" s="2">
-        <v>3.75</v>
+        <v>2.5</v>
       </c>
       <c r="N6" s="2">
-        <v>13.1</v>
-      </c>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15">
+        <v>7.9</v>
+      </c>
+      <c r="O6">
+        <v>8.08</v>
+      </c>
+      <c r="P6">
+        <v>67.650000000000006</v>
+      </c>
+      <c r="Q6">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="R6">
+        <v>20.85</v>
+      </c>
+      <c r="S6">
+        <v>-23.03</v>
+      </c>
+      <c r="T6">
+        <v>-2.0499999999999998</v>
+      </c>
+      <c r="U6">
+        <v>13.49</v>
+      </c>
+      <c r="V6">
+        <v>28.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>800</v>
+        <v>810</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2">
-        <v>61.5</v>
+        <v>42.5</v>
       </c>
       <c r="E7" s="2">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="G7" s="2">
-        <v>6.6</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="H7" s="2">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I7" s="2">
-        <v>7.2</v>
+        <v>7</v>
       </c>
       <c r="J7" s="2">
-        <v>8.3000000000000007</v>
+        <v>6.9</v>
       </c>
       <c r="K7" s="2">
-        <v>1772</v>
+        <v>1778</v>
       </c>
       <c r="L7" s="2">
-        <v>464.6</v>
+        <v>468.2</v>
       </c>
       <c r="M7" s="2">
-        <v>3.2</v>
+        <v>1.75</v>
       </c>
       <c r="N7" s="2">
-        <v>10.5</v>
-      </c>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15">
+        <v>5.5</v>
+      </c>
+      <c r="O7">
+        <v>9.16</v>
+      </c>
+      <c r="P7">
+        <v>66.58</v>
+      </c>
+      <c r="Q7">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="R7">
+        <v>20.74</v>
+      </c>
+      <c r="S7">
+        <v>-28.58</v>
+      </c>
+      <c r="T7">
+        <v>-6.4</v>
+      </c>
+      <c r="U7">
+        <v>14.38</v>
+      </c>
+      <c r="V7">
+        <v>29.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="B8" s="2">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="E8" s="2">
-        <v>20.5</v>
+        <v>135</v>
       </c>
       <c r="F8" s="2">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="G8" s="2">
-        <v>5.75</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="H8" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I8" s="2">
-        <v>7.15</v>
+        <v>7.2</v>
       </c>
       <c r="J8" s="2">
-        <v>7.5</v>
+        <v>9.5</v>
       </c>
       <c r="K8" s="2">
-        <v>1774</v>
+        <v>1765</v>
       </c>
       <c r="L8" s="2">
-        <v>465.9</v>
+        <v>461.5</v>
       </c>
       <c r="M8" s="2">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="N8" s="2">
-        <v>7.9</v>
-      </c>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" spans="1:15">
+        <v>18</v>
+      </c>
+      <c r="O8">
+        <v>12.17</v>
+      </c>
+      <c r="P8">
+        <v>70.040000000000006</v>
+      </c>
+      <c r="Q8">
+        <v>21.6</v>
+      </c>
+      <c r="R8">
+        <v>22.23</v>
+      </c>
+      <c r="S8">
+        <v>-9.43</v>
+      </c>
+      <c r="T8">
+        <v>9.73</v>
+      </c>
+      <c r="U8">
+        <v>13.07</v>
+      </c>
+      <c r="V8">
+        <v>23.74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>6</v>
+        <v>102</v>
       </c>
       <c r="B9" s="2">
-        <v>810</v>
+        <v>800</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
-        <v>42.5</v>
+        <v>87.5</v>
       </c>
       <c r="E9" s="2">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="F9" s="2">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="G9" s="2">
-        <v>4.6500000000000004</v>
+        <v>9.4</v>
       </c>
       <c r="H9" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I9" s="2">
-        <v>7</v>
+        <v>7.3</v>
       </c>
       <c r="J9" s="2">
-        <v>6.9</v>
+        <v>10.1</v>
       </c>
       <c r="K9" s="2">
-        <v>1778</v>
+        <v>1763</v>
       </c>
       <c r="L9" s="2">
-        <v>468.2</v>
+        <v>460</v>
       </c>
       <c r="M9" s="2">
-        <v>1.75</v>
+        <v>6</v>
       </c>
       <c r="N9" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="O9" s="3"/>
-    </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>27.25</v>
+      </c>
+      <c r="O9">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="P9">
+        <v>66.239999999999995</v>
+      </c>
+      <c r="Q9">
+        <v>21.87</v>
+      </c>
+      <c r="R9">
+        <v>22.35</v>
+      </c>
+      <c r="S9">
+        <v>-5.27</v>
+      </c>
+      <c r="T9">
+        <v>-4.3499999999999996</v>
+      </c>
+      <c r="U9">
+        <v>11.82</v>
+      </c>
+      <c r="V9">
+        <v>21.64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>103</v>
+      </c>
+      <c r="B10" s="2">
+        <v>800</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="3"/>
-    </row>
-    <row r="11" spans="1:15">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="D10" s="2">
+        <v>93</v>
+      </c>
+      <c r="E10" s="2">
+        <v>195</v>
+      </c>
+      <c r="F10" s="2">
+        <v>91</v>
+      </c>
+      <c r="G10" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="H10" s="2">
+        <v>118</v>
+      </c>
+      <c r="I10" s="2">
+        <v>7.3</v>
+      </c>
+      <c r="J10" s="2">
+        <v>10.25</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1762</v>
+      </c>
+      <c r="L10" s="2">
+        <v>459</v>
+      </c>
+      <c r="M10" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="N10" s="2">
+        <v>29.5</v>
+      </c>
+      <c r="O10">
+        <v>7.22</v>
+      </c>
+      <c r="P10">
+        <v>64.02</v>
+      </c>
+      <c r="Q10">
+        <v>22.04</v>
+      </c>
+      <c r="R10">
+        <v>22.31</v>
+      </c>
+      <c r="S10">
+        <v>-3.45</v>
+      </c>
+      <c r="T10">
+        <v>-2.2200000000000002</v>
+      </c>
+      <c r="U10">
+        <v>11.58</v>
+      </c>
+      <c r="V10">
+        <v>21.21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>201</v>
+      </c>
+      <c r="B11" s="2">
+        <v>805</v>
+      </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="3"/>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="D11" s="2">
+        <v>98.5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>210</v>
+      </c>
+      <c r="F11" s="2">
+        <v>96</v>
+      </c>
+      <c r="G11" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="H11" s="2">
+        <v>116</v>
+      </c>
+      <c r="I11" s="2">
+        <v>7.25</v>
+      </c>
+      <c r="J11" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1760</v>
+      </c>
+      <c r="L11" s="2">
+        <v>458.5</v>
+      </c>
+      <c r="M11" s="2">
+        <v>7.25</v>
+      </c>
+      <c r="N11" s="2">
+        <v>29.2</v>
+      </c>
+      <c r="O11">
+        <v>14.07</v>
+      </c>
+      <c r="P11">
+        <v>64.319999999999993</v>
+      </c>
+      <c r="Q11">
+        <v>23.16</v>
+      </c>
+      <c r="R11">
+        <v>23.09</v>
+      </c>
+      <c r="S11">
+        <v>-1.1399999999999999</v>
+      </c>
+      <c r="T11">
+        <v>11.76</v>
+      </c>
+      <c r="U11">
+        <v>11.5</v>
+      </c>
+      <c r="V11">
+        <v>22.02</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>1</v>
+        <v>202</v>
       </c>
       <c r="B12" s="2">
-        <v>805</v>
+        <v>830</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
-        <v>81</v>
+        <v>102.5</v>
       </c>
       <c r="E12" s="2">
-        <v>135</v>
+        <v>235</v>
       </c>
       <c r="F12" s="2">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="G12" s="2">
-        <v>8.6999999999999993</v>
+        <v>10.95</v>
       </c>
       <c r="H12" s="2">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I12" s="2">
-        <v>7.2</v>
+        <v>7.4</v>
       </c>
       <c r="J12" s="2">
-        <v>9.5</v>
+        <v>11.2</v>
       </c>
       <c r="K12" s="2">
-        <v>1765</v>
+        <v>1759</v>
       </c>
       <c r="L12" s="2">
-        <v>461.5</v>
+        <v>457.2</v>
       </c>
       <c r="M12" s="2">
-        <v>5</v>
+        <v>7.75</v>
       </c>
       <c r="N12" s="2">
-        <v>18</v>
-      </c>
-      <c r="O12" s="3"/>
-    </row>
-    <row r="13" spans="1:15">
-      <c r="A13" s="2">
-        <v>2</v>
-      </c>
-      <c r="B13" s="2">
-        <v>800</v>
-      </c>
+        <v>29.2</v>
+      </c>
+      <c r="O12">
+        <v>17.23</v>
+      </c>
+      <c r="P12">
+        <v>65.239999999999995</v>
+      </c>
+      <c r="Q12">
+        <v>24.45</v>
+      </c>
+      <c r="R12">
+        <v>24.29</v>
+      </c>
+      <c r="S12">
+        <v>0.84</v>
+      </c>
+      <c r="T12">
+        <v>16.25</v>
+      </c>
+      <c r="U12">
+        <v>11.68</v>
+      </c>
+      <c r="V12">
+        <v>22.89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2">
-        <v>87.5</v>
-      </c>
-      <c r="E13" s="2">
-        <v>175</v>
-      </c>
-      <c r="F13" s="2">
-        <v>86</v>
-      </c>
-      <c r="G13" s="2">
-        <v>9.4</v>
-      </c>
-      <c r="H13" s="2">
-        <v>118</v>
-      </c>
-      <c r="I13" s="2">
-        <v>7.3</v>
-      </c>
-      <c r="J13" s="2">
-        <v>10.1</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1763</v>
-      </c>
-      <c r="L13" s="2">
-        <v>460</v>
-      </c>
-      <c r="M13" s="2">
-        <v>6</v>
-      </c>
-      <c r="N13" s="2">
-        <v>27.25</v>
-      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="2">
-        <v>3</v>
-      </c>
-      <c r="B14" s="2">
-        <v>800</v>
-      </c>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2">
-        <v>93</v>
-      </c>
-      <c r="E14" s="2">
-        <v>195</v>
-      </c>
-      <c r="F14" s="2">
-        <v>91</v>
-      </c>
-      <c r="G14" s="2">
-        <v>9.9</v>
-      </c>
-      <c r="H14" s="2">
-        <v>118</v>
-      </c>
-      <c r="I14" s="2">
-        <v>7.3</v>
-      </c>
-      <c r="J14" s="2">
-        <v>10.25</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1762</v>
-      </c>
-      <c r="L14" s="2">
-        <v>459</v>
-      </c>
-      <c r="M14" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="N14" s="2">
-        <v>29.5</v>
-      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -1067,130 +1434,58 @@
       <c r="N15" s="2"/>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:15">
-      <c r="A16" s="2">
-        <v>4</v>
-      </c>
-      <c r="B16" s="2">
-        <v>805</v>
-      </c>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="2">
-        <v>98.5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>210</v>
-      </c>
-      <c r="F16" s="2">
-        <v>96</v>
-      </c>
-      <c r="G16" s="2">
-        <v>10.5</v>
-      </c>
-      <c r="H16" s="2">
-        <v>116</v>
-      </c>
-      <c r="I16" s="2">
-        <v>7.25</v>
-      </c>
-      <c r="J16" s="2">
-        <v>10.5</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1760</v>
-      </c>
-      <c r="L16" s="2">
-        <v>458.5</v>
-      </c>
-      <c r="M16" s="2">
-        <v>7.25</v>
-      </c>
-      <c r="N16" s="2">
-        <v>29.2</v>
-      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15">
-      <c r="A17" s="2">
-        <v>5</v>
-      </c>
-      <c r="B17" s="2">
-        <v>830</v>
-      </c>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2">
-        <v>102.5</v>
-      </c>
-      <c r="E17" s="2">
-        <v>235</v>
-      </c>
-      <c r="F17" s="2">
-        <v>101</v>
-      </c>
-      <c r="G17" s="2">
-        <v>10.95</v>
-      </c>
-      <c r="H17" s="2">
-        <v>116</v>
-      </c>
-      <c r="I17" s="2">
-        <v>7.4</v>
-      </c>
-      <c r="J17" s="2">
-        <v>11.2</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1759</v>
-      </c>
-      <c r="L17" s="2">
-        <v>457.2</v>
-      </c>
-      <c r="M17" s="2">
-        <v>7.75</v>
-      </c>
-      <c r="N17" s="2">
-        <v>29.2</v>
-      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15">
-      <c r="A18" s="2">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2">
-        <v>870</v>
-      </c>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2">
-        <v>107.5</v>
-      </c>
-      <c r="E18" s="2">
-        <v>265</v>
-      </c>
-      <c r="F18" s="2">
-        <v>106</v>
-      </c>
-      <c r="G18" s="2">
-        <v>11.4</v>
-      </c>
-      <c r="H18" s="2">
-        <v>116</v>
-      </c>
-      <c r="I18" s="2">
-        <v>7.4</v>
-      </c>
-      <c r="J18" s="2">
-        <v>11.4</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1758</v>
-      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1207,7 +1502,7 @@
       <c r="N19" s="2"/>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1224,7 +1519,7 @@
       <c r="N20" s="2"/>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1241,7 +1536,7 @@
       <c r="N21" s="2"/>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1258,7 +1553,7 @@
       <c r="N22" s="2"/>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1275,7 +1570,7 @@
       <c r="N23" s="2"/>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1292,7 +1587,7 @@
       <c r="N24" s="2"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1309,7 +1604,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="3"/>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1326,7 +1621,7 @@
       <c r="N26" s="2"/>
       <c r="O26" s="3"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1343,7 +1638,7 @@
       <c r="N27" s="2"/>
       <c r="O27" s="3"/>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1360,259 +1655,149 @@
       <c r="N28" s="2"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="1:15">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:15">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="3"/>
-    </row>
-    <row r="32" spans="1:15">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="3"/>
-    </row>
-    <row r="33" spans="1:15">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="1:15">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="1:15">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-    </row>
-    <row r="36" spans="1:15">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
-    </row>
-    <row r="37" spans="1:15">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="H1:K1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.9140625" customWidth="1"/>
+    <col min="3" max="3" width="11.97265625" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="11.8359375" customWidth="1"/>
+    <col min="6" max="6" width="12.10546875" customWidth="1"/>
+    <col min="7" max="7" width="10.89453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="7"/>
+      <c r="B1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="9"/>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="45">
-      <c r="A3" s="7"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="9"/>
       <c r="B3" s="4" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1641,7 +1826,7 @@
         <v>24.82</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1670,7 +1855,7 @@
         <v>23.79</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1699,7 +1884,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1728,7 +1913,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1757,7 +1942,7 @@
         <v>28.06</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1786,7 +1971,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1815,7 +2000,7 @@
         <v>23.74</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1844,7 +2029,7 @@
         <v>21.64</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1873,7 +2058,7 @@
         <v>21.21</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1902,7 +2087,7 @@
         <v>22.02</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1931,7 +2116,7 @@
         <v>22.89</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>6</v>
       </c>
@@ -1946,12 +2131,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
R12 Superheated Vapour Data
</commit_message>
<xml_diff>
--- a/THRef/A4_ThRef.xlsx
+++ b/THRef/A4_ThRef.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="41" documentId="11_CF968E0DABCF094F20048FA27BED34BA348958A6" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{80E3B889-913B-4FD4-917A-6B43CB88E818}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_CF968E0DABCF094F20048FA27BED34BA348958A6" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B5B473FE-B43E-470C-A75A-82910F41C054}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="18195" windowHeight="6720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="41">
   <si>
     <t>Run #</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Water Mass flow rate (g/s)</t>
   </si>
   <si>
-    <t>Condenser Temp [C]</t>
-  </si>
-  <si>
     <t>Compressor Speed [rpm]</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>Temperature Compressor Outlet 2</t>
   </si>
   <si>
-    <t>Temperature CompressorOutlet 3</t>
-  </si>
-  <si>
     <t>Temperature Throttle Valve Inlet 4</t>
   </si>
   <si>
@@ -145,6 +139,9 @@
   </si>
   <si>
     <t>Run</t>
+  </si>
+  <si>
+    <t>Temperature Condenser Outlet 3</t>
   </si>
 </sst>
 </file>
@@ -567,823 +564,808 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="E10" sqref="A1:V12"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.91796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.796875" customWidth="1"/>
-    <col min="3" max="3" width="8.33984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.8359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.98828125" customWidth="1"/>
-    <col min="6" max="6" width="10.76171875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.89453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28125" customWidth="1"/>
-    <col min="12" max="12" width="13.5859375" customWidth="1"/>
-    <col min="13" max="13" width="13.1796875" customWidth="1"/>
-    <col min="14" max="14" width="14.390625" customWidth="1"/>
+    <col min="3" max="3" width="11.8359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.98828125" customWidth="1"/>
+    <col min="5" max="5" width="10.76171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.89453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28125" customWidth="1"/>
+    <col min="11" max="11" width="13.5859375" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="14.390625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="68.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="68.25" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>31</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>800</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2">
+        <v>81.3</v>
+      </c>
       <c r="D2" s="2">
-        <v>81.3</v>
+        <v>140</v>
       </c>
       <c r="E2" s="2">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="F2" s="2">
-        <v>80</v>
+        <v>8.9</v>
       </c>
       <c r="G2" s="2">
-        <v>8.9</v>
+        <v>119</v>
       </c>
       <c r="H2" s="2">
-        <v>119</v>
+        <v>7.2</v>
       </c>
       <c r="I2" s="2">
-        <v>7.2</v>
+        <v>9.75</v>
       </c>
       <c r="J2" s="2">
-        <v>9.75</v>
+        <v>1767</v>
       </c>
       <c r="K2" s="2">
-        <v>1767</v>
+        <v>461.3</v>
       </c>
       <c r="L2" s="2">
-        <v>461.3</v>
+        <v>5</v>
       </c>
       <c r="M2" s="2">
-        <v>5</v>
-      </c>
-      <c r="N2" s="2">
         <v>18</v>
       </c>
+      <c r="N2">
+        <v>12.52</v>
+      </c>
       <c r="O2">
-        <v>12.52</v>
+        <v>63.04</v>
       </c>
       <c r="P2">
-        <v>63.04</v>
+        <v>22.33</v>
       </c>
       <c r="Q2">
-        <v>22.33</v>
+        <v>22.45</v>
       </c>
       <c r="R2">
-        <v>22.45</v>
+        <v>-8.85</v>
       </c>
       <c r="S2">
-        <v>-8.85</v>
+        <v>10.5</v>
       </c>
       <c r="T2">
-        <v>10.5</v>
+        <v>12.56</v>
       </c>
       <c r="U2">
-        <v>12.56</v>
-      </c>
-      <c r="V2">
         <v>24.82</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>795</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="2">
+        <v>75.5</v>
+      </c>
       <c r="D3" s="2">
-        <v>75.5</v>
+        <v>115</v>
       </c>
       <c r="E3" s="2">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="F3" s="2">
-        <v>75</v>
+        <v>8.1</v>
       </c>
       <c r="G3" s="2">
-        <v>8.1</v>
+        <v>118</v>
       </c>
       <c r="H3" s="2">
-        <v>118</v>
+        <v>7.2</v>
       </c>
       <c r="I3" s="2">
-        <v>7.2</v>
+        <v>9</v>
       </c>
       <c r="J3" s="2">
-        <v>9</v>
+        <v>1767</v>
       </c>
       <c r="K3" s="2">
-        <v>1767</v>
+        <v>461.9</v>
       </c>
       <c r="L3" s="2">
-        <v>461.9</v>
+        <v>4.5</v>
       </c>
       <c r="M3" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="N3" s="2">
         <v>17.5</v>
       </c>
+      <c r="N3">
+        <v>11.25</v>
+      </c>
       <c r="O3">
-        <v>11.25</v>
+        <v>65.010000000000005</v>
       </c>
       <c r="P3">
-        <v>65.010000000000005</v>
+        <v>20.81</v>
       </c>
       <c r="Q3">
-        <v>20.81</v>
+        <v>21.65</v>
       </c>
       <c r="R3">
-        <v>21.65</v>
+        <v>-11.91</v>
       </c>
       <c r="S3">
-        <v>-11.91</v>
+        <v>7.82</v>
       </c>
       <c r="T3">
-        <v>7.82</v>
+        <v>12.64</v>
       </c>
       <c r="U3">
-        <v>12.64</v>
-      </c>
-      <c r="V3">
         <v>23.79</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>800</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="2">
+        <v>68.5</v>
+      </c>
       <c r="D4" s="2">
-        <v>68.5</v>
+        <v>85</v>
       </c>
       <c r="E4" s="2">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="F4" s="2">
-        <v>68</v>
+        <v>7.4</v>
       </c>
       <c r="G4" s="2">
-        <v>7.4</v>
+        <v>119</v>
       </c>
       <c r="H4" s="2">
-        <v>119</v>
+        <v>7.2</v>
       </c>
       <c r="I4" s="2">
-        <v>7.2</v>
+        <v>8.5</v>
       </c>
       <c r="J4" s="2">
-        <v>8.5</v>
+        <v>1770</v>
       </c>
       <c r="K4" s="2">
-        <v>1770</v>
+        <v>461.45</v>
       </c>
       <c r="L4" s="2">
-        <v>461.45</v>
+        <v>3.75</v>
       </c>
       <c r="M4" s="2">
-        <v>3.75</v>
-      </c>
-      <c r="N4" s="2">
         <v>13.1</v>
       </c>
+      <c r="N4">
+        <v>9.67</v>
+      </c>
       <c r="O4">
-        <v>9.67</v>
+        <v>66.56</v>
       </c>
       <c r="P4">
-        <v>66.56</v>
+        <v>20.72</v>
       </c>
       <c r="Q4">
-        <v>20.72</v>
+        <v>21.37</v>
       </c>
       <c r="R4">
-        <v>21.37</v>
+        <v>-15.8</v>
       </c>
       <c r="S4">
-        <v>-15.8</v>
+        <v>4.24</v>
       </c>
       <c r="T4">
-        <v>4.24</v>
+        <v>12.87</v>
       </c>
       <c r="U4">
-        <v>12.87</v>
-      </c>
-      <c r="V4">
         <v>25.8</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>800</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2">
+        <v>61.5</v>
+      </c>
       <c r="D5" s="2">
-        <v>61.5</v>
+        <v>65</v>
       </c>
       <c r="E5" s="2">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F5" s="2">
-        <v>61</v>
+        <v>6.6</v>
       </c>
       <c r="G5" s="2">
-        <v>6.6</v>
+        <v>119</v>
       </c>
       <c r="H5" s="2">
-        <v>119</v>
+        <v>7.2</v>
       </c>
       <c r="I5" s="2">
-        <v>7.2</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="J5" s="2">
-        <v>8.3000000000000007</v>
+        <v>1772</v>
       </c>
       <c r="K5" s="2">
-        <v>1772</v>
+        <v>464.6</v>
       </c>
       <c r="L5" s="2">
-        <v>464.6</v>
+        <v>3.2</v>
       </c>
       <c r="M5" s="2">
-        <v>3.2</v>
-      </c>
-      <c r="N5" s="2">
         <v>10.5</v>
       </c>
+      <c r="N5">
+        <v>8.31</v>
+      </c>
       <c r="O5">
-        <v>8.31</v>
+        <v>67.510000000000005</v>
       </c>
       <c r="P5">
-        <v>67.510000000000005</v>
+        <v>20.190000000000001</v>
       </c>
       <c r="Q5">
-        <v>20.190000000000001</v>
+        <v>21.05</v>
       </c>
       <c r="R5">
-        <v>21.05</v>
+        <v>-19.239999999999998</v>
       </c>
       <c r="S5">
-        <v>-19.239999999999998</v>
+        <v>1.05</v>
       </c>
       <c r="T5">
-        <v>1.05</v>
+        <v>13.09</v>
       </c>
       <c r="U5">
-        <v>13.09</v>
-      </c>
-      <c r="V5">
         <v>26.7</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>810</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2">
+        <v>53</v>
+      </c>
       <c r="D6" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="E6" s="2">
         <v>53</v>
       </c>
-      <c r="E6" s="2">
-        <v>20.5</v>
-      </c>
       <c r="F6" s="2">
-        <v>53</v>
+        <v>5.75</v>
       </c>
       <c r="G6" s="2">
-        <v>5.75</v>
+        <v>120</v>
       </c>
       <c r="H6" s="2">
-        <v>120</v>
+        <v>7.15</v>
       </c>
       <c r="I6" s="2">
-        <v>7.15</v>
+        <v>7.5</v>
       </c>
       <c r="J6" s="2">
-        <v>7.5</v>
+        <v>1774</v>
       </c>
       <c r="K6" s="2">
-        <v>1774</v>
+        <v>465.9</v>
       </c>
       <c r="L6" s="2">
-        <v>465.9</v>
+        <v>2.5</v>
       </c>
       <c r="M6" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="N6" s="2">
         <v>7.9</v>
       </c>
+      <c r="N6">
+        <v>8.08</v>
+      </c>
       <c r="O6">
-        <v>8.08</v>
+        <v>67.650000000000006</v>
       </c>
       <c r="P6">
-        <v>67.650000000000006</v>
+        <v>19.739999999999998</v>
       </c>
       <c r="Q6">
-        <v>19.739999999999998</v>
+        <v>20.85</v>
       </c>
       <c r="R6">
-        <v>20.85</v>
+        <v>-23.03</v>
       </c>
       <c r="S6">
-        <v>-23.03</v>
+        <v>-2.0499999999999998</v>
       </c>
       <c r="T6">
-        <v>-2.0499999999999998</v>
+        <v>13.49</v>
       </c>
       <c r="U6">
-        <v>13.49</v>
-      </c>
-      <c r="V6">
         <v>28.06</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>810</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2">
+        <v>42.5</v>
+      </c>
       <c r="D7" s="2">
-        <v>42.5</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="F7" s="2">
-        <v>43</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="G7" s="2">
-        <v>4.6500000000000004</v>
+        <v>120</v>
       </c>
       <c r="H7" s="2">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="I7" s="2">
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="J7" s="2">
-        <v>6.9</v>
+        <v>1778</v>
       </c>
       <c r="K7" s="2">
-        <v>1778</v>
+        <v>468.2</v>
       </c>
       <c r="L7" s="2">
-        <v>468.2</v>
+        <v>1.75</v>
       </c>
       <c r="M7" s="2">
-        <v>1.75</v>
-      </c>
-      <c r="N7" s="2">
         <v>5.5</v>
       </c>
+      <c r="N7">
+        <v>9.16</v>
+      </c>
       <c r="O7">
-        <v>9.16</v>
+        <v>66.58</v>
       </c>
       <c r="P7">
-        <v>66.58</v>
+        <v>19.579999999999998</v>
       </c>
       <c r="Q7">
-        <v>19.579999999999998</v>
+        <v>20.74</v>
       </c>
       <c r="R7">
-        <v>20.74</v>
+        <v>-28.58</v>
       </c>
       <c r="S7">
-        <v>-28.58</v>
+        <v>-6.4</v>
       </c>
       <c r="T7">
-        <v>-6.4</v>
+        <v>14.38</v>
       </c>
       <c r="U7">
-        <v>14.38</v>
-      </c>
-      <c r="V7">
         <v>29.6</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>101</v>
       </c>
       <c r="B8" s="2">
         <v>805</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2">
+        <v>81</v>
+      </c>
       <c r="D8" s="2">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="E8" s="2">
-        <v>135</v>
+        <v>80</v>
       </c>
       <c r="F8" s="2">
-        <v>80</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="G8" s="2">
-        <v>8.6999999999999993</v>
+        <v>118</v>
       </c>
       <c r="H8" s="2">
-        <v>118</v>
+        <v>7.2</v>
       </c>
       <c r="I8" s="2">
-        <v>7.2</v>
+        <v>9.5</v>
       </c>
       <c r="J8" s="2">
-        <v>9.5</v>
+        <v>1765</v>
       </c>
       <c r="K8" s="2">
-        <v>1765</v>
+        <v>461.5</v>
       </c>
       <c r="L8" s="2">
-        <v>461.5</v>
+        <v>5</v>
       </c>
       <c r="M8" s="2">
-        <v>5</v>
-      </c>
-      <c r="N8" s="2">
         <v>18</v>
       </c>
+      <c r="N8">
+        <v>12.17</v>
+      </c>
       <c r="O8">
-        <v>12.17</v>
+        <v>70.040000000000006</v>
       </c>
       <c r="P8">
-        <v>70.040000000000006</v>
+        <v>21.6</v>
       </c>
       <c r="Q8">
-        <v>21.6</v>
+        <v>22.23</v>
       </c>
       <c r="R8">
-        <v>22.23</v>
+        <v>-9.43</v>
       </c>
       <c r="S8">
-        <v>-9.43</v>
+        <v>9.73</v>
       </c>
       <c r="T8">
-        <v>9.73</v>
+        <v>13.07</v>
       </c>
       <c r="U8">
-        <v>13.07</v>
-      </c>
-      <c r="V8">
         <v>23.74</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>102</v>
       </c>
       <c r="B9" s="2">
         <v>800</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>87.5</v>
+      </c>
       <c r="D9" s="2">
-        <v>87.5</v>
+        <v>175</v>
       </c>
       <c r="E9" s="2">
-        <v>175</v>
+        <v>86</v>
       </c>
       <c r="F9" s="2">
-        <v>86</v>
+        <v>9.4</v>
       </c>
       <c r="G9" s="2">
-        <v>9.4</v>
+        <v>118</v>
       </c>
       <c r="H9" s="2">
-        <v>118</v>
+        <v>7.3</v>
       </c>
       <c r="I9" s="2">
-        <v>7.3</v>
+        <v>10.1</v>
       </c>
       <c r="J9" s="2">
-        <v>10.1</v>
+        <v>1763</v>
       </c>
       <c r="K9" s="2">
-        <v>1763</v>
+        <v>460</v>
       </c>
       <c r="L9" s="2">
-        <v>460</v>
+        <v>6</v>
       </c>
       <c r="M9" s="2">
-        <v>6</v>
-      </c>
-      <c r="N9" s="2">
         <v>27.25</v>
       </c>
+      <c r="N9">
+        <v>4.5599999999999996</v>
+      </c>
       <c r="O9">
-        <v>4.5599999999999996</v>
+        <v>66.239999999999995</v>
       </c>
       <c r="P9">
-        <v>66.239999999999995</v>
+        <v>21.87</v>
       </c>
       <c r="Q9">
-        <v>21.87</v>
+        <v>22.35</v>
       </c>
       <c r="R9">
-        <v>22.35</v>
+        <v>-5.27</v>
       </c>
       <c r="S9">
-        <v>-5.27</v>
+        <v>-4.3499999999999996</v>
       </c>
       <c r="T9">
-        <v>-4.3499999999999996</v>
+        <v>11.82</v>
       </c>
       <c r="U9">
-        <v>11.82</v>
-      </c>
-      <c r="V9">
         <v>21.64</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>103</v>
       </c>
       <c r="B10" s="2">
         <v>800</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>93</v>
+      </c>
       <c r="D10" s="2">
-        <v>93</v>
+        <v>195</v>
       </c>
       <c r="E10" s="2">
-        <v>195</v>
+        <v>91</v>
       </c>
       <c r="F10" s="2">
-        <v>91</v>
+        <v>9.9</v>
       </c>
       <c r="G10" s="2">
-        <v>9.9</v>
+        <v>118</v>
       </c>
       <c r="H10" s="2">
-        <v>118</v>
+        <v>7.3</v>
       </c>
       <c r="I10" s="2">
-        <v>7.3</v>
+        <v>10.25</v>
       </c>
       <c r="J10" s="2">
-        <v>10.25</v>
+        <v>1762</v>
       </c>
       <c r="K10" s="2">
-        <v>1762</v>
+        <v>459</v>
       </c>
       <c r="L10" s="2">
-        <v>459</v>
+        <v>6.5</v>
       </c>
       <c r="M10" s="2">
-        <v>6.5</v>
-      </c>
-      <c r="N10" s="2">
         <v>29.5</v>
       </c>
+      <c r="N10">
+        <v>7.22</v>
+      </c>
       <c r="O10">
-        <v>7.22</v>
+        <v>64.02</v>
       </c>
       <c r="P10">
-        <v>64.02</v>
+        <v>22.04</v>
       </c>
       <c r="Q10">
-        <v>22.04</v>
+        <v>22.31</v>
       </c>
       <c r="R10">
-        <v>22.31</v>
+        <v>-3.45</v>
       </c>
       <c r="S10">
-        <v>-3.45</v>
+        <v>-2.2200000000000002</v>
       </c>
       <c r="T10">
-        <v>-2.2200000000000002</v>
+        <v>11.58</v>
       </c>
       <c r="U10">
-        <v>11.58</v>
-      </c>
-      <c r="V10">
         <v>21.21</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>201</v>
       </c>
       <c r="B11" s="2">
         <v>805</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2">
+        <v>98.5</v>
+      </c>
       <c r="D11" s="2">
-        <v>98.5</v>
+        <v>210</v>
       </c>
       <c r="E11" s="2">
-        <v>210</v>
+        <v>96</v>
       </c>
       <c r="F11" s="2">
-        <v>96</v>
+        <v>10.5</v>
       </c>
       <c r="G11" s="2">
+        <v>116</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7.25</v>
+      </c>
+      <c r="I11" s="2">
         <v>10.5</v>
       </c>
-      <c r="H11" s="2">
-        <v>116</v>
-      </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
+        <v>1760</v>
+      </c>
+      <c r="K11" s="2">
+        <v>458.5</v>
+      </c>
+      <c r="L11" s="2">
         <v>7.25</v>
       </c>
-      <c r="J11" s="2">
-        <v>10.5</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1760</v>
-      </c>
-      <c r="L11" s="2">
-        <v>458.5</v>
-      </c>
       <c r="M11" s="2">
-        <v>7.25</v>
-      </c>
-      <c r="N11" s="2">
         <v>29.2</v>
       </c>
+      <c r="N11">
+        <v>14.07</v>
+      </c>
       <c r="O11">
-        <v>14.07</v>
+        <v>64.319999999999993</v>
       </c>
       <c r="P11">
-        <v>64.319999999999993</v>
+        <v>23.16</v>
       </c>
       <c r="Q11">
-        <v>23.16</v>
+        <v>23.09</v>
       </c>
       <c r="R11">
-        <v>23.09</v>
+        <v>-1.1399999999999999</v>
       </c>
       <c r="S11">
-        <v>-1.1399999999999999</v>
+        <v>11.76</v>
       </c>
       <c r="T11">
-        <v>11.76</v>
+        <v>11.5</v>
       </c>
       <c r="U11">
-        <v>11.5</v>
-      </c>
-      <c r="V11">
         <v>22.02</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>202</v>
       </c>
       <c r="B12" s="2">
         <v>830</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2">
+        <v>102.5</v>
+      </c>
       <c r="D12" s="2">
-        <v>102.5</v>
+        <v>235</v>
       </c>
       <c r="E12" s="2">
-        <v>235</v>
+        <v>101</v>
       </c>
       <c r="F12" s="2">
-        <v>101</v>
+        <v>10.95</v>
       </c>
       <c r="G12" s="2">
-        <v>10.95</v>
+        <v>116</v>
       </c>
       <c r="H12" s="2">
-        <v>116</v>
+        <v>7.4</v>
       </c>
       <c r="I12" s="2">
-        <v>7.4</v>
+        <v>11.2</v>
       </c>
       <c r="J12" s="2">
-        <v>11.2</v>
+        <v>1759</v>
       </c>
       <c r="K12" s="2">
-        <v>1759</v>
+        <v>457.2</v>
       </c>
       <c r="L12" s="2">
-        <v>457.2</v>
+        <v>7.75</v>
       </c>
       <c r="M12" s="2">
-        <v>7.75</v>
-      </c>
-      <c r="N12" s="2">
         <v>29.2</v>
       </c>
+      <c r="N12">
+        <v>17.23</v>
+      </c>
       <c r="O12">
-        <v>17.23</v>
+        <v>65.239999999999995</v>
       </c>
       <c r="P12">
-        <v>65.239999999999995</v>
+        <v>24.45</v>
       </c>
       <c r="Q12">
-        <v>24.45</v>
+        <v>24.29</v>
       </c>
       <c r="R12">
-        <v>24.29</v>
+        <v>0.84</v>
       </c>
       <c r="S12">
-        <v>0.84</v>
+        <v>16.25</v>
       </c>
       <c r="T12">
-        <v>16.25</v>
+        <v>11.68</v>
       </c>
       <c r="U12">
-        <v>11.68</v>
-      </c>
-      <c r="V12">
         <v>22.89</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1397,10 +1379,9 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="3"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1414,10 +1395,9 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="3"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1431,10 +1411,9 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="3"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1448,10 +1427,9 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1465,10 +1443,9 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="3"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1482,10 +1459,9 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="3"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1499,10 +1475,9 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="3"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1516,10 +1491,9 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1533,10 +1507,9 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1550,10 +1523,9 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1567,10 +1539,9 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="3"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1584,10 +1555,9 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="3"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1601,10 +1571,9 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
-      <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1618,10 +1587,9 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1635,10 +1603,9 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1652,10 +1619,9 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
-      <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N28" s="3"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1669,9 +1635,8 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1685,9 +1650,8 @@
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1701,7 +1665,6 @@
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>